<commit_message>
Bulk Commit to update
</commit_message>
<xml_diff>
--- a/docs/man_tests_T1A2.xlsx
+++ b/docs/man_tests_T1A2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shelbyd/CODING/Projects/Ruby/CA_Terminal_App_RPSLS/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A8B799-143C-D84A-A2CA-D53D7A8482BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1BC44F-3761-A145-B8CA-138E48C315D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-4060" windowWidth="28440" windowHeight="17540" xr2:uid="{E4B1E5C7-DAD6-3D4D-9E2A-0CE9718F5B2E}"/>
+    <workbookView xWindow="-36720" yWindow="-4060" windowWidth="28440" windowHeight="17540" xr2:uid="{E4B1E5C7-DAD6-3D4D-9E2A-0CE9718F5B2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
   <si>
     <t>Feature being tested</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>Would equal as "y' returns :begin</t>
+  </si>
+  <si>
+    <t>This test was archived for now as the score board (seperated class)  feature is benched.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discontinued </t>
   </si>
 </sst>
 </file>
@@ -294,7 +300,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +319,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -326,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -350,6 +362,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -668,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB52CDC-51B2-5744-8C62-74681603DE00}">
   <dimension ref="A2:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,7 +1149,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>7</v>
       </c>
@@ -1153,14 +1168,17 @@
       <c r="F31" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>32</v>
+      <c r="G31" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="H31" s="8">
         <v>43944</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>